<commit_message>
arrow on time scale
</commit_message>
<xml_diff>
--- a/data/extraction_grid.xlsx
+++ b/data/extraction_grid.xlsx
@@ -2063,9 +2063,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="W1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="W41" sqref="W41"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5073,7 +5073,7 @@
         <v>2011</v>
       </c>
       <c r="I40" s="18">
-        <v>2050</v>
+        <v>2154</v>
       </c>
       <c r="J40" s="27"/>
       <c r="K40" s="27"/>

</xml_diff>

<commit_message>
plot kevin health outcome
</commit_message>
<xml_diff>
--- a/data/extraction_grid.xlsx
+++ b/data/extraction_grid.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="322">
   <si>
     <t>The public health implications of the Paris Agreement: a modelling study</t>
   </si>
@@ -1042,6 +1042,9 @@
   </si>
   <si>
     <t>publi_yr</t>
+  </si>
+  <si>
+    <t>Microsimulation model</t>
   </si>
 </sst>
 </file>
@@ -1098,6 +1101,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -2107,9 +2111,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D54" sqref="D54"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="AB1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AD8" sqref="AD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2799,7 +2803,7 @@
         <v>219</v>
       </c>
       <c r="AD8" s="39" t="s">
-        <v>211</v>
+        <v>321</v>
       </c>
       <c r="AE8" s="18"/>
     </row>
@@ -5079,7 +5083,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="37" spans="1:31" s="44" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:31" s="44" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="43" t="s">
         <v>119</v>
       </c>

</xml_diff>